<commit_message>
UI tweaks, Address section updated
</commit_message>
<xml_diff>
--- a/Laszlo_Papp/01_Inputs/biz_pricingV2.0.xlsx
+++ b/Laszlo_Papp/01_Inputs/biz_pricingV2.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://innoveo.sharepoint.com/sites/TeamGlobal/Shared Documents/Innoveo Projects/After Training Exercise/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git Repos\Training sandbox\Laszlo_Papp\01_Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{21819EE4-5198-4261-A147-50EC23B47303}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{14DF0E0C-5301-46D0-9638-56F273F2483D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF64E31C-571D-4962-9BFC-A2486EB0B9D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pricing" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>vehicle factor</t>
   </si>
@@ -97,6 +99,33 @@
   </si>
   <si>
     <t>Premium items</t>
+  </si>
+  <si>
+    <t>vehicle year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of use </t>
+  </si>
+  <si>
+    <t>Personal:1 Company:2</t>
+  </si>
+  <si>
+    <t>Car (neworused)</t>
+  </si>
+  <si>
+    <t>New:0, used:1</t>
+  </si>
+  <si>
+    <t>Fuel type</t>
+  </si>
+  <si>
+    <t>Number of drivers, 1,2</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -621,26 +650,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:N12"/>
+  <dimension ref="B2:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -654,7 +683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1">
         <v>2000</v>
       </c>
@@ -680,7 +709,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="K4" t="s">
         <v>18</v>
       </c>
@@ -694,7 +723,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="K5" t="s">
         <v>19</v>
       </c>
@@ -711,7 +740,7 @@
         <v>537.5</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
@@ -749,7 +778,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
         <v>1</v>
       </c>
@@ -781,8 +810,8 @@
         <v>912.5</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>0</v>
       </c>
@@ -791,13 +820,55 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="12" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="4">
         <f>IF(B7=1,2,1.2)*(((ABS(C7-50)/100)+IF(D7&lt;&gt;210,0.2,0)+((E7-1000)/100))+IF(B7=2,((ABS(F7-50)/100)+IF(G7&lt;&gt;210,0.2,0)+((H7-1000)/100)),0))</f>
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="K13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="K14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="K15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="K16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K20" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -816,6 +887,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokumentum" ma:contentTypeID="0x01010099CDED3ECB2B4843831D8747C02ED9CF" ma:contentTypeVersion="10" ma:contentTypeDescription="Új dokumentum létrehozása." ma:contentTypeScope="" ma:versionID="76a815337efc6a58b2e8bd6b7d520bd1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ffabfc81-e8aa-46c0-b37e-f3d37c1335ad" xmlns:ns3="c1503785-5146-4d31-9a3a-ab405e6c3296" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae8f8b2acb53c9f89b3f048a00ead611" ns2:_="" ns3:_="">
     <xsd:import namespace="ffabfc81-e8aa-46c0-b37e-f3d37c1335ad"/>
@@ -1018,15 +1098,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB9DE6E5-223C-4942-81EB-6CE82110EEA9}">
   <ds:schemaRefs>
@@ -1045,6 +1116,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81C3500B-5B04-4CC7-AB8D-AFAC94BC70F0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07D0617-CEE1-4E18-9D77-03E633BA8470}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1061,12 +1140,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81C3500B-5B04-4CC7-AB8D-AFAC94BC70F0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>